<commit_message>
One Page Summary adjustment
</commit_message>
<xml_diff>
--- a/Flow chart.xlsx
+++ b/Flow chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dutch\Documents\WashU Data Bootcamp\07-Project-1\Project_1_Group_5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA079A04-C856-4676-8718-9C2E70214DAE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02A2BE6-E599-48B8-9DDD-CF36DBF11D29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{582C1833-4C58-4DAB-96E8-B51EABC11D9B}"/>
   </bookViews>
@@ -31,11 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>ata1</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -92,15 +88,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>373380</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>335280</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -180,7 +176,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>Remove when $'s missing</a:t>
+            <a:t>Remove when missing price</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100">
             <a:solidFill>
@@ -194,15 +190,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>49530</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>49530</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -250,15 +246,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -302,6 +298,22 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>MERGE</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> &amp; </a:t>
+          </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100">
               <a:solidFill>
@@ -345,15 +357,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
+      <xdr:col>6</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>53764</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>15664</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -403,8 +415,21 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>START 2</a:t>
-          </a:r>
+            <a:t>QUESTION</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> 2</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -412,15 +437,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>198120</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>510540</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -506,15 +531,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>175260</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -530,8 +555,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="175260" y="1668780"/>
-          <a:ext cx="2186940" cy="502920"/>
+          <a:off x="2623653" y="1709253"/>
+          <a:ext cx="2194436" cy="511915"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartInputOutput">
           <a:avLst/>
@@ -584,6 +609,30 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
+            <a:t>YELP API:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>  </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t>20</a:t>
           </a:r>
           <a:r>
@@ -610,24 +659,6 @@
             </a:rPr>
             <a:t>Businesses per ZIP</a:t>
           </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> Code (YELP API)</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
       </xdr:txBody>
@@ -636,15 +667,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -714,7 +745,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>3 Reviews</a:t>
+            <a:t>YELP APIL 3 Reviews</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0">
@@ -726,15 +757,8 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> per busines (YELP API)</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US">
-            <a:effectLst/>
-          </a:endParaRPr>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
+            <a:t> per buss.</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -742,16 +766,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>487680</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>91440</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>300304</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>105431</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>516161</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>55214</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -766,8 +790,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2316480" y="3505200"/>
-          <a:ext cx="2042160" cy="502920"/>
+          <a:off x="2748697" y="3665595"/>
+          <a:ext cx="2052153" cy="511914"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartInputOutput">
           <a:avLst/>
@@ -810,15 +834,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>601980</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>175260</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -903,15 +927,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>60030</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>52596</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>341970</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>67836</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -971,15 +995,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>295149</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>112819</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>201001</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>52596</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1027,15 +1051,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>46482</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1083,16 +1107,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>496824</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>310946</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>177509</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>99060</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>174011</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1110,12 +1134,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4154424" y="3284220"/>
-          <a:ext cx="722376" cy="472440"/>
+          <a:off x="4595635" y="3362919"/>
+          <a:ext cx="2749545" cy="558633"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 61603"/>
+            <a:gd name="adj1" fmla="val 89980"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -1141,15 +1165,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>335280</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>235458</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>163830</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1197,15 +1221,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>47413</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>47413</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1253,15 +1277,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>47413</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>15664</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>55034</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1310,15 +1334,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>339090</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>53340</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>346710</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>175260</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1366,15 +1390,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>270603</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>128797</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>262983</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>75457</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1426,15 +1450,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>266793</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>339090</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>75666</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1484,15 +1508,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>339090</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>434433</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>75666</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1541,67 +1565,17 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>450138</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>109281</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>51432</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>124522</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="108" name="Picture 107">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78455ECC-F902-4499-879D-FA8B88138670}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4743358" y="5684891"/>
-          <a:ext cx="827927" cy="386948"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>13</xdr:col>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>438243</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>128797</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>430623</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>75457</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1653,16 +1627,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>500453</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>90697</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>416632</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>75457</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>75456</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1670,6 +1644,56 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A1CB8A0-AFC4-494B-8642-2B504A44E7E5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6020307" y="5666307"/>
+          <a:ext cx="529497" cy="356467"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>472068</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>81404</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>388249</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>66163</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="120" name="Picture 119">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CD61CF1-967D-4606-B9B3-3B111A0AFCE6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1691,56 +1715,6 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6020307" y="5666307"/>
-          <a:ext cx="529497" cy="356467"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>472068</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>81404</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>388249</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>66164</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="120" name="Picture 119">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CD61CF1-967D-4606-B9B3-3B111A0AFCE6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
           <a:off x="6605239" y="5657014"/>
           <a:ext cx="529497" cy="356467"/>
         </a:xfrm>
@@ -1753,153 +1727,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>62095</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>74083</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="121" name="Flowchart: Terminator 120">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25F8FFEF-D382-4FBC-AC90-6C20AD6C62DA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="7037917" y="6539095"/>
-          <a:ext cx="1322916" cy="371821"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartTerminator">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent3">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>QUESTION</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> 2</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>266792</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>127104</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>333374</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>62095</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="123" name="Connector: Elbow 122">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D1A8D02-1BA4-4513-BE1D-1839F1205000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="95" idx="2"/>
-          <a:endCxn id="121" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="7121796" y="5961517"/>
-          <a:ext cx="474741" cy="680415"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 63669"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>153143</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>60030</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>163831</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -1947,73 +1783,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>127103</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>434434</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>62094</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="158" name="Connector: Elbow 157">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9B0E94A-0ACD-4F00-95D7-C001B663E927}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="115" idx="2"/>
-          <a:endCxn id="121" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1" flipV="1">
-          <a:off x="7819450" y="5944278"/>
-          <a:ext cx="474741" cy="714892"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 63669"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>30480</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>84242</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>10582</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2111,15 +1889,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>339091</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>447888</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>84241</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -2169,16 +1947,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>379730</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>63075</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>600710</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>169332</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>342255</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>50583</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>563235</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>156840</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2193,8 +1971,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11428730" y="5280658"/>
-          <a:ext cx="2062480" cy="646007"/>
+          <a:off x="12584222" y="5484517"/>
+          <a:ext cx="2057275" cy="668389"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartInputOutput">
           <a:avLst/>
@@ -2238,15 +2016,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>243097</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>62200</xdr:rowOff>
+      <xdr:colOff>218111</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>37217</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>235478</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>8860</xdr:rowOff>
+      <xdr:colOff>210492</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>171254</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2261,8 +2039,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10678264" y="6359283"/>
-          <a:ext cx="1220047" cy="1026160"/>
+          <a:off x="10623783" y="7719676"/>
+          <a:ext cx="1216578" cy="1070922"/>
         </a:xfrm>
         <a:prstGeom prst="wave">
           <a:avLst/>
@@ -2298,22 +2076,138 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>179917</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>-1</xdr:rowOff>
+      <xdr:colOff>447020</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>10581</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>275167</xdr:colOff>
-      <xdr:row>45</xdr:row>
-      <xdr:rowOff>11987</xdr:rowOff>
+      <xdr:colOff>259142</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>85318</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="179" name="Connector: Elbow 178">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6ED41A8-679A-45B2-8800-76597AB0D291}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="163" idx="4"/>
+          <a:endCxn id="80" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="11146106" y="5900610"/>
+          <a:ext cx="449491" cy="1036319"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 47221"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>259142</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>156841</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>553066</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>85320</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="182" name="Connector: Elbow 181">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2621FA22-CD4B-4F9E-8032-8E20E6584C82}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="167" idx="3"/>
+          <a:endCxn id="80" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="12402767" y="5639151"/>
+          <a:ext cx="490610" cy="1518121"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>10584</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>546101</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="177" name="Flowchart: Terminator 176">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45F12073-B070-4624-B273-77D9910A2483}"/>
+        <xdr:cNvPr id="187" name="Flowchart: Terminator 186">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{003D7084-5CB9-4FA3-A603-9001A0F55D79}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2321,8 +2215,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10615084" y="7736416"/>
-          <a:ext cx="1322916" cy="371821"/>
+          <a:off x="11789833" y="4148667"/>
+          <a:ext cx="1032935" cy="321733"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartTerminator">
           <a:avLst/>
@@ -2377,195 +2271,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>447888</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>10581</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>239289</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>10552</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="179" name="Connector: Elbow 178">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6ED41A8-679A-45B2-8800-76597AB0D291}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="163" idx="4"/>
-          <a:endCxn id="168" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="10508894" y="5708158"/>
-          <a:ext cx="539721" cy="1019068"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 45958"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>239288</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>169332</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>590889</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>10553</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="182" name="Connector: Elbow 181">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2621FA22-CD4B-4F9E-8032-8E20E6584C82}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="167" idx="3"/>
-          <a:endCxn id="168" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="11490561" y="5724392"/>
-          <a:ext cx="560888" cy="965434"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 49884"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>227542</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>60506</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>239288</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>-1</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="185" name="Straight Arrow Connector 184">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE362537-E3BB-4716-9011-416E95D0E80A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="168" idx="2"/>
-          <a:endCxn id="177" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="11276542" y="7257173"/>
-          <a:ext cx="11746" cy="479243"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>10584</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>546101</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>495155</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>516609</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="187" name="Flowchart: Terminator 186">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{003D7084-5CB9-4FA3-A603-9001A0F55D79}"/>
+        <xdr:cNvPr id="188" name="Flowchart: Terminator 187">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA33A545-51EF-44C9-8C3B-F77080B46822}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2573,8 +2295,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11789833" y="4148667"/>
-          <a:ext cx="1032935" cy="321733"/>
+          <a:off x="495155" y="63500"/>
+          <a:ext cx="1245651" cy="336654"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartTerminator">
           <a:avLst/>
@@ -2607,7 +2329,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>START</a:t>
+            <a:t>QUESTION</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0">
@@ -2615,7 +2337,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> 3</a:t>
+            <a:t> 1</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100">
             <a:solidFill>
@@ -2629,95 +2351,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>603248</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>408515</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="188" name="Flowchart: Terminator 187">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA33A545-51EF-44C9-8C3B-F77080B46822}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="603248" y="63500"/>
-          <a:ext cx="1032934" cy="321733"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartTerminator">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent3">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>START</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t> 1</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>42332</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>52922</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>354752</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>7202</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2778,18 +2420,6 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>YELP</a:t>
-          </a:r>
-          <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="lt1"/>
@@ -2799,7 +2429,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> Data Businesses.JSON</a:t>
+            <a:t>Domino Datalab: Businesses.JSON</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
@@ -2815,15 +2445,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>35983</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>46571</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>348403</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>851</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2893,7 +2523,31 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>YELP Data Reivews.JSON</a:t>
+            <a:t>Domino</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> Datalab:</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="lt1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> Reivews.JSON</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
@@ -2909,15 +2563,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>42332</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>103718</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>354752</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>57998</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -2978,18 +2632,6 @@
             <a:defRPr/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>YELP</a:t>
-          </a:r>
-          <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="lt1"/>
@@ -2999,7 +2641,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> Data Users.JSON</a:t>
+            <a:t>Domino Datalab: Users.JSON</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
@@ -3016,15 +2658,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>179917</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>105834</xdr:rowOff>
+      <xdr:colOff>449705</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>5899</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>172298</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>52494</xdr:rowOff>
+      <xdr:colOff>574623</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>139937</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3039,8 +2681,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2021417" y="4603751"/>
-          <a:ext cx="1220048" cy="1026160"/>
+          <a:off x="1673902" y="5814588"/>
+          <a:ext cx="1349114" cy="1070923"/>
         </a:xfrm>
         <a:prstGeom prst="wave">
           <a:avLst/>
@@ -3075,16 +2717,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>505458</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>57998</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>504593</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>57997</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>176107</xdr:colOff>
+      <xdr:colOff>511606</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>54188</xdr:rowOff>
+      <xdr:rowOff>62456</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3097,17 +2739,17 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="191" idx="4"/>
-          <a:endCxn id="197" idx="0"/>
+          <a:endCxn id="96" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="1067646" y="3168226"/>
-          <a:ext cx="1615440" cy="1512149"/>
+          <a:off x="980558" y="3379540"/>
+          <a:ext cx="1503475" cy="1231210"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 75393"/>
+            <a:gd name="adj1" fmla="val 80742"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -3134,15 +2776,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>176109</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>167639</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>83652</xdr:colOff>
+      <xdr:colOff>511605</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>55214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>509066</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>54187</xdr:rowOff>
+      <xdr:rowOff>62457</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3155,17 +2797,17 @@
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
           <a:stCxn id="44" idx="3"/>
-          <a:endCxn id="197" idx="0"/>
+          <a:endCxn id="96" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="3726731" y="2850600"/>
-          <a:ext cx="786131" cy="2976710"/>
+          <a:off x="2674042" y="3851367"/>
+          <a:ext cx="569374" cy="1221658"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 49435"/>
+            <a:gd name="adj1" fmla="val 50000"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -3191,15 +2833,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>505459</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>504592</xdr:colOff>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>505882</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>505883</xdr:colOff>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>52922</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3218,8 +2860,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="1119292" y="385233"/>
-          <a:ext cx="423" cy="387356"/>
+          <a:off x="1116690" y="400154"/>
+          <a:ext cx="1291" cy="402276"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3247,15 +2889,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>499110</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>7202</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>505459</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>46571</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3303,15 +2945,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>499110</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>851</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>505459</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>103718</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -3359,23 +3001,339 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>40302</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>29635</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>84241</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="219" name="Connector: Elbow 218">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32ED646F-46ED-491A-A76B-6153A4FD436F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="187" idx="2"/>
+          <a:endCxn id="163" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="11282089" y="4277612"/>
+          <a:ext cx="831425" cy="1217000"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 38544"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>30501</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>146695</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>50583</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="223" name="Connector: Elbow 222">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0573347D-FFD6-41EE-9879-6120B6A9FA1C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="187" idx="2"/>
+          <a:endCxn id="167" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="12525130" y="4396787"/>
+          <a:ext cx="835068" cy="1340391"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 39529"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>127003</xdr:colOff>
+      <xdr:colOff>524656</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>105833</xdr:rowOff>
+      <xdr:rowOff>177135</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>499672</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>155609</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C3AAD71D-DA1A-4831-AFF8-3C5BA627D864}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1748853" y="6173201"/>
+          <a:ext cx="587114" cy="353228"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>562133</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>174885</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>222253</xdr:colOff>
+      <xdr:colOff>524657</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>117821</xdr:rowOff>
+      <xdr:rowOff>158149</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9E2A2AE-A7AF-40E0-B149-52676D63C916}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2398428" y="6170951"/>
+          <a:ext cx="574622" cy="358018"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>537148</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>74951</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>562132</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>124916</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Picture 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{096D5BCD-CC1F-4C9F-83C6-9AEF3643DD47}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7270230" y="5696262"/>
+          <a:ext cx="637082" cy="424721"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>462196</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>12491</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>8249</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>48333</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFC03B50-F70D-4745-B189-66D7A71C7BEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10867868" y="8069704"/>
+          <a:ext cx="762000" cy="410595"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>385016</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>113381</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>377397</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>60041</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="215" name="Flowchart: Terminator 214">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{97E4A2B4-7D7E-4EA3-959E-0DC58FFE0137}"/>
+        <xdr:cNvPr id="75" name="Wave 74">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{50B0EBFC-D426-4CE3-B174-C699A37C8463}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3383,24 +3341,84 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1968503" y="6043083"/>
-          <a:ext cx="1322917" cy="371821"/>
-        </a:xfrm>
-        <a:prstGeom prst="flowChartTerminator">
+          <a:off x="12014885" y="7795840"/>
+          <a:ext cx="1216578" cy="1070922"/>
+        </a:xfrm>
+        <a:prstGeom prst="wave">
           <a:avLst/>
         </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent3">
+          <a:schemeClr val="accent1">
             <a:shade val="50000"/>
           </a:schemeClr>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent3"/>
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>522032</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>85319</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>608350</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>62459</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="80" name="Rectangle 79">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84595BF4-D176-4E35-B1C3-FF0C6798F2A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10927704" y="6643516"/>
+          <a:ext cx="1922613" cy="726648"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="lt1"/>
@@ -3417,21 +3435,217 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>QUESTION</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0">
+            <a:t>STATISTICAL ANALYSIS</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>214303</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>62459</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>259143</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>171082</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="38" name="Connector: Elbow 37">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07EB5F22-C079-429D-B88D-156EC51AEC35}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="80" idx="2"/>
+          <a:endCxn id="168" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="11318854" y="7283383"/>
+          <a:ext cx="483377" cy="656939"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 43957"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>259142</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>62458</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>381207</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>59868</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="46" name="Connector: Elbow 45">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D4889C8-5CAB-43C3-A6A1-C03FE40CE3A1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="80" idx="2"/>
+          <a:endCxn id="75" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="11976322" y="7282852"/>
+          <a:ext cx="559541" cy="734163"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 38190"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>162396</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>62457</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>248714</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>39597</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="96" name="Rectangle 95">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DB73EFC-89E4-40B7-97D2-A1C51788C290}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1386593" y="4746883"/>
+          <a:ext cx="1922613" cy="726648"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
               <a:solidFill>
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t> 1</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100">
-            <a:solidFill>
-              <a:sysClr val="windowText" lastClr="000000"/>
-            </a:solidFill>
-          </a:endParaRPr>
+            <a:t>STATISTICAL ANALYSIS:</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>T-Test Male/Female</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>T-Test Gender/Rating</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3440,34 +3654,34 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>174629</xdr:colOff>
+      <xdr:colOff>511605</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>104141</xdr:rowOff>
+      <xdr:rowOff>39597</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>176108</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>105833</xdr:rowOff>
+      <xdr:colOff>512164</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>139764</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="217" name="Straight Arrow Connector 216">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{077CFDC1-7E26-4319-BA2B-7F753275E41C}"/>
+        <xdr:cNvPr id="54" name="Straight Arrow Connector 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F612FC7C-14DA-46AB-A795-EEA96E575BA9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="197" idx="2"/>
-          <a:endCxn id="215" idx="0"/>
+          <a:stCxn id="96" idx="2"/>
+          <a:endCxn id="197" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="2629962" y="5501641"/>
-          <a:ext cx="1479" cy="541442"/>
+        <a:xfrm>
+          <a:off x="2347900" y="5473531"/>
+          <a:ext cx="559" cy="474922"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3493,120 +3707,54 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>40302</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>29635</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>84241</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="219" name="Connector: Elbow 218">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32ED646F-46ED-491A-A76B-6153A4FD436F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="187" idx="2"/>
-          <a:endCxn id="163" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="5400000">
-          <a:off x="11282089" y="4277612"/>
-          <a:ext cx="831425" cy="1217000"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 38544"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>29634</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>389551</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>63075</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="223" name="Connector: Elbow 222">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0573347D-FFD6-41EE-9879-6120B6A9FA1C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="187" idx="2"/>
-          <a:endCxn id="167" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="12388047" y="4388654"/>
-          <a:ext cx="810258" cy="973750"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector3">
-          <a:avLst>
-            <a:gd name="adj1" fmla="val 39551"/>
-          </a:avLst>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
+      <xdr:colOff>14375</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>75483</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>217715</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>100642</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="72" name="Picture 71">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1408F4BC-9321-4EA4-941A-B4B1E8488DC3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12695205" y="8299332"/>
+          <a:ext cx="807189" cy="398970"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -3909,20 +4057,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C28205-495A-4364-BBC0-514F6DD6447F}">
-  <dimension ref="V30"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="61" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="53" workbookViewId="0">
+      <selection activeCell="X50" sqref="X50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="30" spans="22:22" x14ac:dyDescent="0.3">
-      <c r="V30" t="s">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
A lot of monkeying around and cleaning up to get it right - rolling my eyes -
</commit_message>
<xml_diff>
--- a/Flow chart.xlsx
+++ b/Flow chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dutch\Documents\WashU Data Bootcamp\07-Project-1\Project_1_Group_5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02A2BE6-E599-48B8-9DDD-CF36DBF11D29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A29BAA-613B-4827-912F-A053023601D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{582C1833-4C58-4DAB-96E8-B51EABC11D9B}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,10 +29,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1139,7 +1136,7 @@
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 89980"/>
+            <a:gd name="adj1" fmla="val 89449"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -1861,7 +1858,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>List of Review</a:t>
+            <a:t>List of Reviews</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0">
@@ -1873,7 +1870,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t> count by gender by ZIP Code (.csv</a:t>
+            <a:t>  by gender by ZIP Code .CSV</a:t>
           </a:r>
           <a:endParaRPr lang="en-US">
             <a:effectLst/>
@@ -2001,11 +1998,19 @@
           <a:pPr algn="l"/>
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Data</a:t>
+            <a:t>CENSUS</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> per zipcode about economical data (Census API)</a:t>
+            <a:t> API: </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Economical Data</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> per zipcode  </a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1100"/>
         </a:p>
@@ -2076,15 +2081,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>447020</xdr:colOff>
+      <xdr:colOff>442895</xdr:colOff>
       <xdr:row>34</xdr:row>
-      <xdr:rowOff>10581</xdr:rowOff>
+      <xdr:rowOff>10582</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>259142</xdr:colOff>
+      <xdr:colOff>263267</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>85318</xdr:rowOff>
+      <xdr:rowOff>70942</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2102,12 +2107,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="11146106" y="5900610"/>
-          <a:ext cx="449491" cy="1036319"/>
+          <a:off x="11609127" y="6068425"/>
+          <a:ext cx="434172" cy="1028070"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 47221"/>
+            <a:gd name="adj1" fmla="val 50000"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -2134,15 +2139,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>259142</xdr:colOff>
+      <xdr:colOff>263268</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>156841</xdr:rowOff>
+      <xdr:rowOff>156839</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>553066</xdr:colOff>
+      <xdr:colOff>551418</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>85320</xdr:rowOff>
+      <xdr:rowOff>70941</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2160,12 +2165,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="12402767" y="5639151"/>
-          <a:ext cx="490610" cy="1518121"/>
+          <a:off x="12850763" y="5814212"/>
+          <a:ext cx="474819" cy="1495848"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 50000"/>
+            <a:gd name="adj1" fmla="val 53028"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -2659,14 +2664,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>449705</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>5899</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>106535</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>574623</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>139937</xdr:rowOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>53667</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2681,8 +2686,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1673902" y="5814588"/>
-          <a:ext cx="1349114" cy="1070923"/>
+          <a:off x="2261252" y="7208950"/>
+          <a:ext cx="1332616" cy="1068566"/>
         </a:xfrm>
         <a:prstGeom prst="wave">
           <a:avLst/>
@@ -2718,15 +2723,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>504593</xdr:colOff>
+      <xdr:colOff>500466</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>57997</xdr:rowOff>
+      <xdr:rowOff>57998</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>511606</xdr:colOff>
+      <xdr:colOff>507479</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>62456</xdr:rowOff>
+      <xdr:rowOff>76829</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2744,12 +2749,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="980558" y="3379540"/>
-          <a:ext cx="1503475" cy="1231210"/>
+          <a:off x="1558482" y="3571982"/>
+          <a:ext cx="1514076" cy="1214711"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 80742"/>
+            <a:gd name="adj1" fmla="val 80386"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -2776,15 +2781,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>511605</xdr:colOff>
+      <xdr:colOff>507480</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>55214</xdr:rowOff>
+      <xdr:rowOff>55215</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>509066</xdr:colOff>
+      <xdr:colOff>507417</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>62457</xdr:rowOff>
+      <xdr:rowOff>76830</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2802,8 +2807,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="2674042" y="3851367"/>
-          <a:ext cx="569374" cy="1221658"/>
+          <a:off x="3235528" y="4041393"/>
+          <a:ext cx="582332" cy="1207635"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
@@ -3119,14 +3124,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>524656</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>177135</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>90867</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>499672</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>155609</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>69340</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3155,8 +3160,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1748853" y="6173201"/>
-          <a:ext cx="587114" cy="353228"/>
+          <a:off x="2336203" y="7567093"/>
+          <a:ext cx="578865" cy="352285"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3169,14 +3174,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>562133</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>174885</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>88617</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
       <xdr:colOff>524657</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>158149</xdr:rowOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>64260</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3205,8 +3210,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2398428" y="6170951"/>
-          <a:ext cx="574622" cy="358018"/>
+          <a:off x="2977529" y="7564843"/>
+          <a:ext cx="566373" cy="349455"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3380,13 +3385,13 @@
       <xdr:col>18</xdr:col>
       <xdr:colOff>522032</xdr:colOff>
       <xdr:row>36</xdr:row>
-      <xdr:rowOff>85319</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>608350</xdr:colOff>
+      <xdr:rowOff>70942</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>4501</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>62459</xdr:rowOff>
+      <xdr:rowOff>48082</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3401,8 +3406,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10927704" y="6643516"/>
-          <a:ext cx="1922613" cy="726648"/>
+          <a:off x="11391315" y="6799546"/>
+          <a:ext cx="1897865" cy="724762"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3435,6 +3440,17 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
+            <a:t>MERGE by zip</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>STATISTICAL ANALYSIS</a:t>
           </a:r>
         </a:p>
@@ -3445,15 +3461,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>214303</xdr:colOff>
+      <xdr:colOff>214302</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>62459</xdr:rowOff>
+      <xdr:rowOff>48082</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>259143</xdr:colOff>
+      <xdr:colOff>263267</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>171082</xdr:rowOff>
+      <xdr:rowOff>170788</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3471,12 +3487,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="5400000">
-          <a:off x="11318854" y="7283383"/>
-          <a:ext cx="483377" cy="656939"/>
+          <a:off x="11765582" y="7446160"/>
+          <a:ext cx="496518" cy="652814"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 43957"/>
+            <a:gd name="adj1" fmla="val 47683"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -3503,15 +3519,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>259142</xdr:colOff>
+      <xdr:colOff>263267</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>62458</xdr:rowOff>
+      <xdr:rowOff>48081</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>381207</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>59868</xdr:rowOff>
+      <xdr:rowOff>59987</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3529,12 +3545,12 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm rot="16200000" flipH="1">
-          <a:off x="11976322" y="7282852"/>
-          <a:ext cx="559541" cy="734163"/>
+          <a:off x="12414831" y="7449724"/>
+          <a:ext cx="572623" cy="721789"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector3">
           <a:avLst>
-            <a:gd name="adj1" fmla="val 38190"/>
+            <a:gd name="adj1" fmla="val 42010"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
@@ -3563,13 +3579,13 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>162396</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>62457</xdr:rowOff>
+      <xdr:rowOff>76829</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>248714</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>39597</xdr:rowOff>
+      <xdr:rowOff>53969</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3584,8 +3600,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1386593" y="4746883"/>
-          <a:ext cx="1922613" cy="726648"/>
+          <a:off x="1973943" y="4936376"/>
+          <a:ext cx="1897865" cy="724763"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3618,22 +3634,7 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>STATISTICAL ANALYSIS:</a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:sysClr val="windowText" lastClr="000000"/>
-              </a:solidFill>
-            </a:rPr>
-            <a:t>T-Test Male/Female</a:t>
+            <a:t>MERGE:</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -3644,8 +3645,21 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
-            <a:t>T-Test Gender/Rating</a:t>
-          </a:r>
+            <a:t>reviewer</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> data with gender</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3654,15 +3668,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>511605</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>39597</xdr:rowOff>
+      <xdr:colOff>501729</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>120105</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>512164</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>139764</xdr:rowOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>53200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3674,14 +3688,14 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="96" idx="2"/>
+          <a:stCxn id="56" idx="2"/>
           <a:endCxn id="197" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2347900" y="5473531"/>
-          <a:ext cx="559" cy="474922"/>
+          <a:off x="2917125" y="6848709"/>
+          <a:ext cx="10435" cy="493812"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3755,6 +3769,155 @@
         </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>156645</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>142965</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>242963</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>120105</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="56" name="Rectangle 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA394C5C-661D-447A-BAFB-2D2BAA31B148}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1968192" y="6123946"/>
+          <a:ext cx="1897865" cy="724763"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent4">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent4"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent4"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>STATISTICAL ANALYSIS:</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>T-Test Male/Female</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>T-Test Gender/Rating</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>501729</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>53969</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>507480</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>142965</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Straight Arrow Connector 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C800C596-B99F-4165-9851-80B3CF1C6B7E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="96" idx="2"/>
+          <a:endCxn id="56" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2917125" y="5661139"/>
+          <a:ext cx="5751" cy="462807"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4060,7 +4223,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="53" workbookViewId="0">
-      <selection activeCell="X50" sqref="X50"/>
+      <selection activeCell="AL12" sqref="AL12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>